<commit_message>
updated daily log from June
</commit_message>
<xml_diff>
--- a/data/phenological_monitoring.xlsx
+++ b/data/phenological_monitoring.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58B2D24-A37C-C64F-B3DF-CC8B839919F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70077468-CF7E-9144-9280-669BA2FDD24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3886" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3890" uniqueCount="678">
   <si>
     <t>tree_ID</t>
   </si>
@@ -2952,11 +2952,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W631"/>
+  <dimension ref="A1:X631"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W2" sqref="W2"/>
+    <sheetView tabSelected="1" topLeftCell="A593" zoomScale="132" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X606" sqref="X606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2965,7 +2965,7 @@
     <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3035,8 +3035,11 @@
       <c r="W1" s="1">
         <v>155</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X1" s="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -3104,7 +3107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3172,7 +3175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -3240,7 +3243,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -3308,7 +3311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -3376,7 +3379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -3444,7 +3447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -3512,7 +3515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -3580,7 +3583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -3648,7 +3651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -3716,7 +3719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -3784,7 +3787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -3852,7 +3855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -3920,7 +3923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -3988,7 +3991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -14945,7 +14948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="177" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>193</v>
       </c>
@@ -15013,7 +15016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>194</v>
       </c>
@@ -15081,7 +15084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>195</v>
       </c>
@@ -15149,7 +15152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>196</v>
       </c>
@@ -15217,7 +15220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>197</v>
       </c>
@@ -15285,7 +15288,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>198</v>
       </c>
@@ -15352,8 +15355,11 @@
       <c r="W182" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="183" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X182" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>201</v>
       </c>
@@ -15420,8 +15426,11 @@
       <c r="W183">
         <v>4</v>
       </c>
-    </row>
-    <row r="184" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X183">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>202</v>
       </c>
@@ -15488,8 +15497,11 @@
       <c r="W184" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="185" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X184" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>203</v>
       </c>
@@ -15556,8 +15568,11 @@
       <c r="W185">
         <v>4</v>
       </c>
-    </row>
-    <row r="186" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X185">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>204</v>
       </c>
@@ -15627,8 +15642,11 @@
       <c r="W186" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="187" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X186" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>206</v>
       </c>
@@ -15695,8 +15713,11 @@
       <c r="W187">
         <v>4</v>
       </c>
-    </row>
-    <row r="188" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X187">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>207</v>
       </c>
@@ -15763,8 +15784,11 @@
       <c r="W188" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="189" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X188" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>208</v>
       </c>
@@ -15831,8 +15855,11 @@
       <c r="W189" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="190" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X189" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>209</v>
       </c>
@@ -15902,8 +15929,11 @@
       <c r="W190" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="191" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X190" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>210</v>
       </c>
@@ -15970,8 +16000,11 @@
       <c r="W191" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="192" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X191" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>211</v>
       </c>
@@ -16039,7 +16072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>212</v>
       </c>
@@ -16107,7 +16140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>213</v>
       </c>
@@ -16178,7 +16211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>215</v>
       </c>
@@ -16246,7 +16279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>216</v>
       </c>
@@ -16314,7 +16347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>217</v>
       </c>
@@ -16381,8 +16414,11 @@
       <c r="W197" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="198" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X197" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>218</v>
       </c>
@@ -16452,8 +16488,11 @@
       <c r="W198">
         <v>3</v>
       </c>
-    </row>
-    <row r="199" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X198">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>220</v>
       </c>
@@ -16520,8 +16559,11 @@
       <c r="W199" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="200" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X199" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>221</v>
       </c>
@@ -16591,8 +16633,11 @@
       <c r="W200">
         <v>4</v>
       </c>
-    </row>
-    <row r="201" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X200">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>222</v>
       </c>
@@ -16659,8 +16704,11 @@
       <c r="W201" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="202" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X201" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>223</v>
       </c>
@@ -16727,8 +16775,11 @@
       <c r="W202">
         <v>3</v>
       </c>
-    </row>
-    <row r="203" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X202" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>224</v>
       </c>
@@ -16795,8 +16846,11 @@
       <c r="W203" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="204" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X203" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>225</v>
       </c>
@@ -16863,8 +16917,11 @@
       <c r="W204">
         <v>4</v>
       </c>
-    </row>
-    <row r="205" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X204" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>226</v>
       </c>
@@ -16934,8 +16991,11 @@
       <c r="W205" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="206" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X205" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="206" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>227</v>
       </c>
@@ -17002,8 +17062,11 @@
       <c r="W206">
         <v>4</v>
       </c>
-    </row>
-    <row r="207" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X206">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>228</v>
       </c>
@@ -17070,8 +17133,11 @@
       <c r="W207" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="208" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X207" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>229</v>
       </c>
@@ -17141,8 +17207,11 @@
       <c r="W208">
         <v>4</v>
       </c>
-    </row>
-    <row r="209" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X208" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>230</v>
       </c>
@@ -17209,8 +17278,11 @@
       <c r="W209" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="210" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X209" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>231</v>
       </c>
@@ -17277,8 +17349,11 @@
       <c r="W210">
         <v>3</v>
       </c>
-    </row>
-    <row r="211" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X210" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="211" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>232</v>
       </c>
@@ -17348,8 +17423,11 @@
       <c r="W211" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="212" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X211" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>233</v>
       </c>
@@ -17416,8 +17494,11 @@
       <c r="W212" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="213" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X212" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>234</v>
       </c>
@@ -17484,8 +17565,11 @@
       <c r="W213">
         <v>3</v>
       </c>
-    </row>
-    <row r="214" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X213">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>235</v>
       </c>
@@ -17552,8 +17636,11 @@
       <c r="W214" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="215" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X214" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="215" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>236</v>
       </c>
@@ -17620,8 +17707,11 @@
       <c r="W215">
         <v>3</v>
       </c>
-    </row>
-    <row r="216" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X215">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>237</v>
       </c>
@@ -17691,8 +17781,11 @@
       <c r="W216" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="217" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X216" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="217" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>238</v>
       </c>
@@ -17759,8 +17852,11 @@
       <c r="W217">
         <v>4</v>
       </c>
-    </row>
-    <row r="218" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X217" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="218" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>239</v>
       </c>
@@ -17827,8 +17923,11 @@
       <c r="W218" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="219" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X218" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>240</v>
       </c>
@@ -17895,8 +17994,11 @@
       <c r="W219">
         <v>4</v>
       </c>
-    </row>
-    <row r="220" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X219" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>241</v>
       </c>
@@ -17963,8 +18065,11 @@
       <c r="W220" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="221" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X220" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="221" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>242</v>
       </c>
@@ -18031,8 +18136,11 @@
       <c r="W221">
         <v>4</v>
       </c>
-    </row>
-    <row r="222" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X221">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>243</v>
       </c>
@@ -18099,8 +18207,11 @@
       <c r="W222" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="223" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X222" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>244</v>
       </c>
@@ -18170,8 +18281,11 @@
       <c r="W223">
         <v>3</v>
       </c>
-    </row>
-    <row r="224" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X223" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="224" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>245</v>
       </c>
@@ -18238,8 +18352,11 @@
       <c r="W224" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="225" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X224" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>246</v>
       </c>
@@ -18309,8 +18426,11 @@
       <c r="W225">
         <v>4</v>
       </c>
-    </row>
-    <row r="226" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X225" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="226" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>247</v>
       </c>
@@ -18377,8 +18497,11 @@
       <c r="W226" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="227" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X226" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="227" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>248</v>
       </c>
@@ -18445,8 +18568,11 @@
       <c r="W227">
         <v>4</v>
       </c>
-    </row>
-    <row r="228" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X227">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="228" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>249</v>
       </c>
@@ -18513,8 +18639,11 @@
       <c r="W228" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="229" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X228" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="229" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>250</v>
       </c>
@@ -18581,8 +18710,11 @@
       <c r="W229" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="230" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X229" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="230" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>251</v>
       </c>
@@ -18649,8 +18781,11 @@
       <c r="W230" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="231" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X230" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>252</v>
       </c>
@@ -18717,8 +18852,11 @@
       <c r="W231" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="232" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X231" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="232" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>253</v>
       </c>
@@ -18785,8 +18923,11 @@
       <c r="W232" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="233" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X232" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="233" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>254</v>
       </c>
@@ -18853,8 +18994,11 @@
       <c r="W233" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="234" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X233" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="234" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>255</v>
       </c>
@@ -18921,8 +19065,11 @@
       <c r="W234" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="235" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X234" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="235" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>256</v>
       </c>
@@ -18989,8 +19136,11 @@
       <c r="W235" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="236" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X235" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="236" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>257</v>
       </c>
@@ -19057,8 +19207,11 @@
       <c r="W236" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="237" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X236" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="237" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>258</v>
       </c>
@@ -19125,8 +19278,11 @@
       <c r="W237">
         <v>4</v>
       </c>
-    </row>
-    <row r="238" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X237" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>259</v>
       </c>
@@ -19193,8 +19349,11 @@
       <c r="W238" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="239" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X238" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>260</v>
       </c>
@@ -19261,8 +19420,11 @@
       <c r="W239" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="240" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X239" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="240" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>261</v>
       </c>
@@ -19329,8 +19491,11 @@
       <c r="W240" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="241" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X240" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="241" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>262</v>
       </c>
@@ -19397,8 +19562,11 @@
       <c r="W241" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="242" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X241" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="242" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>263</v>
       </c>
@@ -19465,8 +19633,11 @@
       <c r="W242" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="243" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X242" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="243" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>264</v>
       </c>
@@ -19533,8 +19704,11 @@
       <c r="W243">
         <v>4</v>
       </c>
-    </row>
-    <row r="244" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X243" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="244" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>265</v>
       </c>
@@ -19601,8 +19775,11 @@
       <c r="W244" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="245" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X244" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="245" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>266</v>
       </c>
@@ -19669,8 +19846,11 @@
       <c r="W245">
         <v>4</v>
       </c>
-    </row>
-    <row r="246" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X245" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="246" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>267</v>
       </c>
@@ -19737,8 +19917,11 @@
       <c r="W246" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="247" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X246" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="247" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>268</v>
       </c>
@@ -19805,8 +19988,11 @@
       <c r="W247" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="248" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X247" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="248" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>269</v>
       </c>
@@ -19873,8 +20059,11 @@
       <c r="W248" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="249" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X248" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="249" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>270</v>
       </c>
@@ -19941,8 +20130,11 @@
       <c r="W249" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="250" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X249" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="250" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>271</v>
       </c>
@@ -20009,8 +20201,11 @@
       <c r="W250" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="251" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X250" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="251" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>272</v>
       </c>
@@ -20077,8 +20272,11 @@
       <c r="W251">
         <v>4</v>
       </c>
-    </row>
-    <row r="252" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X251" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="252" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>273</v>
       </c>
@@ -20145,8 +20343,11 @@
       <c r="W252" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="253" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X252" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>274</v>
       </c>
@@ -20213,8 +20414,11 @@
       <c r="W253" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="254" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X253" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="254" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>275</v>
       </c>
@@ -20281,8 +20485,11 @@
       <c r="W254" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="255" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X254" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="255" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>276</v>
       </c>
@@ -20349,8 +20556,11 @@
       <c r="W255" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="256" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X255" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="256" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
         <v>277</v>
       </c>
@@ -20417,8 +20627,11 @@
       <c r="W256" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="257" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X256" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="257" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>278</v>
       </c>
@@ -20485,8 +20698,11 @@
       <c r="W257">
         <v>4</v>
       </c>
-    </row>
-    <row r="258" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X257">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="258" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>279</v>
       </c>
@@ -20553,8 +20769,11 @@
       <c r="W258">
         <v>4</v>
       </c>
-    </row>
-    <row r="259" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X258" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="259" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
         <v>280</v>
       </c>
@@ -20621,8 +20840,11 @@
       <c r="W259" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="260" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X259" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="260" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>281</v>
       </c>
@@ -20689,8 +20911,11 @@
       <c r="W260" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="261" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X260" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="261" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>282</v>
       </c>
@@ -20757,8 +20982,11 @@
       <c r="W261" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="262" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X261" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="262" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>283</v>
       </c>
@@ -20825,8 +21053,11 @@
       <c r="W262" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="263" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X262" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="263" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
         <v>284</v>
       </c>
@@ -20893,8 +21124,11 @@
       <c r="W263" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="264" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X263" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="264" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>285</v>
       </c>
@@ -20961,8 +21195,11 @@
       <c r="W264" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="265" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X264" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="265" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
         <v>286</v>
       </c>
@@ -21029,8 +21266,11 @@
       <c r="W265" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="266" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X265" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="266" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>287</v>
       </c>
@@ -21097,8 +21337,11 @@
       <c r="W266" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="267" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X266" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="267" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
         <v>288</v>
       </c>
@@ -21165,8 +21408,11 @@
       <c r="W267" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="268" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X267" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="268" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>289</v>
       </c>
@@ -21233,8 +21479,11 @@
       <c r="W268" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="269" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X268" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="269" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
         <v>290</v>
       </c>
@@ -21301,8 +21550,11 @@
       <c r="W269" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="270" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X269" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="270" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>291</v>
       </c>
@@ -21369,8 +21621,11 @@
       <c r="W270" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="271" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X270" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="271" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
         <v>292</v>
       </c>
@@ -21437,8 +21692,11 @@
       <c r="W271" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="272" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X271" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="272" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>293</v>
       </c>
@@ -33531,7 +33789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="449" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
         <v>486</v>
       </c>
@@ -33599,7 +33857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="450" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A450" s="1" t="s">
         <v>487</v>
       </c>
@@ -33667,7 +33925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="451" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
         <v>488</v>
       </c>
@@ -33735,7 +33993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="452" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A452" s="1" t="s">
         <v>489</v>
       </c>
@@ -33802,8 +34060,11 @@
       <c r="W452" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="453" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X452" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="453" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
         <v>492</v>
       </c>
@@ -33870,8 +34131,11 @@
       <c r="W453" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="454" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X453" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="454" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A454" s="1" t="s">
         <v>493</v>
       </c>
@@ -33938,8 +34202,11 @@
       <c r="W454" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="455" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X454" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="455" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
         <v>494</v>
       </c>
@@ -34006,8 +34273,11 @@
       <c r="W455" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="456" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X455" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="456" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A456" s="1" t="s">
         <v>495</v>
       </c>
@@ -34074,8 +34344,11 @@
       <c r="W456" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="457" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X456" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="457" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
         <v>496</v>
       </c>
@@ -34145,8 +34418,11 @@
       <c r="W457">
         <v>4</v>
       </c>
-    </row>
-    <row r="458" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X457" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="458" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A458" s="1" t="s">
         <v>497</v>
       </c>
@@ -34213,8 +34489,11 @@
       <c r="W458" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="459" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X458" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="459" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
         <v>498</v>
       </c>
@@ -34281,8 +34560,11 @@
       <c r="W459" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="460" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X459" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="460" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A460" s="1" t="s">
         <v>499</v>
       </c>
@@ -34349,8 +34631,11 @@
       <c r="W460" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="461" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X460" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="461" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
         <v>500</v>
       </c>
@@ -34417,8 +34702,11 @@
       <c r="W461" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="462" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X461" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="462" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A462" s="1" t="s">
         <v>501</v>
       </c>
@@ -34485,8 +34773,11 @@
       <c r="W462" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="463" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X462" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="463" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
         <v>502</v>
       </c>
@@ -34553,8 +34844,11 @@
       <c r="W463" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="464" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X463" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="464" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A464" s="1" t="s">
         <v>503</v>
       </c>
@@ -34621,8 +34915,11 @@
       <c r="W464" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="465" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X464" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="465" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
         <v>504</v>
       </c>
@@ -34689,8 +34986,11 @@
       <c r="W465" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="466" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X465" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="466" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
         <v>505</v>
       </c>
@@ -34757,8 +35057,11 @@
       <c r="W466" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="467" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X466" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="467" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A467" s="1" t="s">
         <v>506</v>
       </c>
@@ -34825,8 +35128,11 @@
       <c r="W467" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="468" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X467" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="468" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
         <v>507</v>
       </c>
@@ -34896,8 +35202,11 @@
       <c r="W468">
         <v>3</v>
       </c>
-    </row>
-    <row r="469" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X468">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="469" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A469" s="1" t="s">
         <v>508</v>
       </c>
@@ -34967,8 +35276,11 @@
       <c r="W469" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="470" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X469" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="470" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
         <v>509</v>
       </c>
@@ -35035,8 +35347,11 @@
       <c r="W470">
         <v>4</v>
       </c>
-    </row>
-    <row r="471" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X470">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="471" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A471" s="1" t="s">
         <v>510</v>
       </c>
@@ -35103,8 +35418,11 @@
       <c r="W471" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="472" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X471" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="472" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
         <v>511</v>
       </c>
@@ -35171,8 +35489,11 @@
       <c r="W472">
         <v>4</v>
       </c>
-    </row>
-    <row r="473" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X472">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="473" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A473" s="1" t="s">
         <v>512</v>
       </c>
@@ -35239,8 +35560,11 @@
       <c r="W473" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="474" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X473" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="474" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
         <v>513</v>
       </c>
@@ -35307,8 +35631,11 @@
       <c r="W474" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="475" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X474">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="475" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A475" s="1" t="s">
         <v>514</v>
       </c>
@@ -35378,8 +35705,11 @@
       <c r="W475" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="476" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X475" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="476" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
         <v>515</v>
       </c>
@@ -35446,8 +35776,11 @@
       <c r="W476" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="477" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X476">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="477" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A477" s="1" t="s">
         <v>516</v>
       </c>
@@ -35514,8 +35847,11 @@
       <c r="W477" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="478" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X477" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="478" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
         <v>517</v>
       </c>
@@ -35582,8 +35918,11 @@
       <c r="W478">
         <v>4</v>
       </c>
-    </row>
-    <row r="479" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X478" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="479" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A479" s="1" t="s">
         <v>518</v>
       </c>
@@ -35650,8 +35989,11 @@
       <c r="W479" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="480" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X479" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="480" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
         <v>519</v>
       </c>
@@ -35718,8 +36060,11 @@
       <c r="W480" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="481" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X480" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="481" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A481" s="1" t="s">
         <v>520</v>
       </c>
@@ -35786,8 +36131,11 @@
       <c r="W481" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="482" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X481" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="482" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
         <v>521</v>
       </c>
@@ -35854,8 +36202,11 @@
       <c r="W482" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="483" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X482" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="483" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A483" s="1" t="s">
         <v>522</v>
       </c>
@@ -35922,8 +36273,11 @@
       <c r="W483" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="484" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X483" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="484" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
         <v>523</v>
       </c>
@@ -35990,8 +36344,11 @@
       <c r="W484" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="485" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X484" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="485" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A485" s="1" t="s">
         <v>524</v>
       </c>
@@ -36058,8 +36415,11 @@
       <c r="W485" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="486" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X485" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="486" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A486" t="s">
         <v>525</v>
       </c>
@@ -36126,8 +36486,11 @@
       <c r="W486" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="487" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X486">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="487" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A487" s="1" t="s">
         <v>526</v>
       </c>
@@ -36194,8 +36557,11 @@
       <c r="W487" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="488" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X487" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="488" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A488" t="s">
         <v>527</v>
       </c>
@@ -36265,8 +36631,11 @@
       <c r="W488" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="489" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X488">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="489" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A489" t="s">
         <v>528</v>
       </c>
@@ -36333,8 +36702,11 @@
       <c r="W489" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="490" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X489">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="490" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A490" s="1" t="s">
         <v>529</v>
       </c>
@@ -36401,8 +36773,11 @@
       <c r="W490" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="491" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X490" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="491" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
         <v>530</v>
       </c>
@@ -36469,8 +36844,11 @@
       <c r="W491" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="492" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X491">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="492" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A492" s="1" t="s">
         <v>531</v>
       </c>
@@ -36537,8 +36915,11 @@
       <c r="W492" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="493" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X492" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="493" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
         <v>532</v>
       </c>
@@ -36605,8 +36986,11 @@
       <c r="W493" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="494" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X493" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="494" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A494" s="1" t="s">
         <v>533</v>
       </c>
@@ -36673,8 +37057,11 @@
       <c r="W494" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="495" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X494" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="495" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
         <v>534</v>
       </c>
@@ -36744,8 +37131,11 @@
       <c r="W495" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="496" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X495" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="496" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A496" s="1" t="s">
         <v>536</v>
       </c>
@@ -36812,8 +37202,11 @@
       <c r="W496" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="497" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X496" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="497" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A497" t="s">
         <v>537</v>
       </c>
@@ -36880,8 +37273,11 @@
       <c r="W497">
         <v>4</v>
       </c>
-    </row>
-    <row r="498" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X497" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="498" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A498" s="1" t="s">
         <v>538</v>
       </c>
@@ -36948,8 +37344,11 @@
       <c r="W498" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="499" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X498" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="499" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A499" t="s">
         <v>539</v>
       </c>
@@ -37016,8 +37415,11 @@
       <c r="W499" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="500" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X499" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="500" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A500" s="1" t="s">
         <v>540</v>
       </c>
@@ -37084,8 +37486,11 @@
       <c r="W500" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="501" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X500" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="501" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
         <v>541</v>
       </c>
@@ -37152,8 +37557,11 @@
       <c r="W501" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="502" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X501" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="502" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A502" s="1" t="s">
         <v>542</v>
       </c>
@@ -37220,8 +37628,11 @@
       <c r="W502" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="503" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X502" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="503" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A503" t="s">
         <v>543</v>
       </c>
@@ -37288,8 +37699,11 @@
       <c r="W503" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="504" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X503" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="504" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A504" s="1" t="s">
         <v>544</v>
       </c>
@@ -37356,8 +37770,11 @@
       <c r="W504" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="505" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X504" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="505" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A505" t="s">
         <v>545</v>
       </c>
@@ -37424,8 +37841,11 @@
       <c r="W505" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="506" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X505" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="506" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A506" s="1" t="s">
         <v>546</v>
       </c>
@@ -37492,8 +37912,11 @@
       <c r="W506" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="507" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X506" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="507" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A507" t="s">
         <v>547</v>
       </c>
@@ -37560,8 +37983,11 @@
       <c r="W507">
         <v>4</v>
       </c>
-    </row>
-    <row r="508" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X507" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="508" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A508" s="1" t="s">
         <v>548</v>
       </c>
@@ -37628,8 +38054,11 @@
       <c r="W508" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="509" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X508" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="509" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A509" t="s">
         <v>549</v>
       </c>
@@ -37696,8 +38125,11 @@
       <c r="W509" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="510" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X509" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="510" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A510" s="1" t="s">
         <v>550</v>
       </c>
@@ -37764,8 +38196,11 @@
       <c r="W510" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="511" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X510" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="511" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A511" t="s">
         <v>551</v>
       </c>
@@ -37832,8 +38267,11 @@
       <c r="W511" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="512" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X511" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="512" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A512" s="1" t="s">
         <v>552</v>
       </c>
@@ -37900,8 +38338,11 @@
       <c r="W512" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="513" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X512" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="513" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A513" t="s">
         <v>553</v>
       </c>
@@ -37968,8 +38409,11 @@
       <c r="W513" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="514" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X513" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="514" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A514" s="1" t="s">
         <v>554</v>
       </c>
@@ -38036,8 +38480,11 @@
       <c r="W514" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="515" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X514" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="515" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A515" t="s">
         <v>555</v>
       </c>
@@ -38104,8 +38551,11 @@
       <c r="W515" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="516" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X515" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="516" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A516" s="1" t="s">
         <v>556</v>
       </c>
@@ -38172,8 +38622,11 @@
       <c r="W516" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="517" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X516" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="517" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A517" t="s">
         <v>557</v>
       </c>
@@ -38243,8 +38696,11 @@
       <c r="W517">
         <v>1</v>
       </c>
-    </row>
-    <row r="518" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X517">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="518" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A518" s="1" t="s">
         <v>558</v>
       </c>
@@ -38314,8 +38770,11 @@
       <c r="W518" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="519" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X518" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="519" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A519" t="s">
         <v>560</v>
       </c>
@@ -38382,8 +38841,11 @@
       <c r="W519">
         <v>4</v>
       </c>
-    </row>
-    <row r="520" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X519">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="520" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A520" s="1" t="s">
         <v>561</v>
       </c>
@@ -38450,8 +38912,11 @@
       <c r="W520" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="521" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X520" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="521" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A521" t="s">
         <v>562</v>
       </c>
@@ -38518,8 +38983,11 @@
       <c r="W521">
         <v>4</v>
       </c>
-    </row>
-    <row r="522" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X521">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="522" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A522" s="1" t="s">
         <v>563</v>
       </c>
@@ -38586,8 +39054,11 @@
       <c r="W522" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="523" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X522" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="523" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A523" t="s">
         <v>564</v>
       </c>
@@ -38654,8 +39125,11 @@
       <c r="W523" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="524" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X523" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="524" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A524" s="1" t="s">
         <v>565</v>
       </c>
@@ -38722,8 +39196,11 @@
       <c r="W524" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="525" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X524" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="525" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A525" t="s">
         <v>566</v>
       </c>
@@ -38790,8 +39267,11 @@
       <c r="W525" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="526" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X525" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="526" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A526" s="1" t="s">
         <v>567</v>
       </c>
@@ -38858,8 +39338,11 @@
       <c r="W526" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="527" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X526" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="527" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A527" t="s">
         <v>568</v>
       </c>
@@ -38926,8 +39409,11 @@
       <c r="W527">
         <v>4</v>
       </c>
-    </row>
-    <row r="528" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X527" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="528" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A528" s="1" t="s">
         <v>569</v>
       </c>
@@ -38997,8 +39483,11 @@
       <c r="W528" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="529" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X528" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="529" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
         <v>570</v>
       </c>
@@ -39065,8 +39554,11 @@
       <c r="W529" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="530" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X529" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="530" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A530" s="1" t="s">
         <v>571</v>
       </c>
@@ -39133,8 +39625,11 @@
       <c r="W530" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="531" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X530" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="531" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A531" t="s">
         <v>572</v>
       </c>
@@ -39201,8 +39696,11 @@
       <c r="W531" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="532" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X531" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="532" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A532" s="1" t="s">
         <v>573</v>
       </c>
@@ -39272,8 +39770,11 @@
       <c r="W532" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="533" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X532" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="533" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A533" t="s">
         <v>574</v>
       </c>
@@ -39340,8 +39841,11 @@
       <c r="W533" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="534" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X533" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="534" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A534" s="1" t="s">
         <v>575</v>
       </c>
@@ -39408,8 +39912,11 @@
       <c r="W534" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="535" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X534" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="535" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A535" t="s">
         <v>576</v>
       </c>
@@ -39476,8 +39983,11 @@
       <c r="W535" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="536" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X535" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="536" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A536" t="s">
         <v>577</v>
       </c>
@@ -39544,8 +40054,11 @@
       <c r="W536" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="537" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X536" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="537" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A537" s="1" t="s">
         <v>578</v>
       </c>
@@ -39612,8 +40125,11 @@
       <c r="W537" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="538" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X537" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="538" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A538" t="s">
         <v>579</v>
       </c>
@@ -39680,8 +40196,11 @@
       <c r="W538" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="539" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X538" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="539" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A539" s="1" t="s">
         <v>580</v>
       </c>
@@ -39748,8 +40267,11 @@
       <c r="W539" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="540" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X539" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="540" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
         <v>581</v>
       </c>
@@ -39816,8 +40338,11 @@
       <c r="W540" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="541" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X540" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="541" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A541" s="1" t="s">
         <v>582</v>
       </c>
@@ -39884,8 +40409,11 @@
       <c r="W541" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="542" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X541" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="542" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A542" t="s">
         <v>583</v>
       </c>
@@ -39952,8 +40480,11 @@
       <c r="W542">
         <v>1</v>
       </c>
-    </row>
-    <row r="543" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X542">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="543" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A543" s="1" t="s">
         <v>586</v>
       </c>
@@ -40020,8 +40551,11 @@
       <c r="W543" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="544" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X543" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="544" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
         <v>587</v>
       </c>
@@ -40088,8 +40622,11 @@
       <c r="W544">
         <v>1</v>
       </c>
-    </row>
-    <row r="545" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X544">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="545" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A545" s="1" t="s">
         <v>588</v>
       </c>
@@ -40156,8 +40693,11 @@
       <c r="W545" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="546" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X545" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="546" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A546" t="s">
         <v>589</v>
       </c>
@@ -40224,8 +40764,11 @@
       <c r="W546">
         <v>1</v>
       </c>
-    </row>
-    <row r="547" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X546">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="547" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A547" s="1" t="s">
         <v>590</v>
       </c>
@@ -40293,7 +40836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="548" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="548" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A548" t="s">
         <v>591</v>
       </c>
@@ -40361,7 +40904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="549" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="549" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A549" s="1" t="s">
         <v>592</v>
       </c>
@@ -40429,7 +40972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="550" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="550" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A550" t="s">
         <v>593</v>
       </c>
@@ -40497,7 +41040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="551" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="551" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A551" s="1" t="s">
         <v>594</v>
       </c>
@@ -40565,7 +41108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="552" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="552" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A552" t="s">
         <v>595</v>
       </c>
@@ -40633,7 +41176,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="553" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="553" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A553" s="1" t="s">
         <v>596</v>
       </c>
@@ -40701,7 +41244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="554" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="554" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A554" t="s">
         <v>597</v>
       </c>
@@ -40769,7 +41312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="555" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="555" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A555" s="1" t="s">
         <v>598</v>
       </c>
@@ -40837,7 +41380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="556" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="556" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A556" t="s">
         <v>599</v>
       </c>
@@ -40905,7 +41448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="557" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="557" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A557" s="1" t="s">
         <v>600</v>
       </c>
@@ -40973,7 +41516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="558" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="558" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A558" t="s">
         <v>601</v>
       </c>
@@ -41041,7 +41584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="559" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="559" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A559" t="s">
         <v>602</v>
       </c>
@@ -41109,7 +41652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="560" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="560" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A560" s="1" t="s">
         <v>603</v>
       </c>
@@ -43353,7 +43896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="593" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="593" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A593" t="s">
         <v>636</v>
       </c>
@@ -43421,7 +43964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="594" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="594" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A594" s="1" t="s">
         <v>637</v>
       </c>
@@ -43489,7 +44032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="595" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="595" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A595" t="s">
         <v>638</v>
       </c>
@@ -43557,7 +44100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="596" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="596" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A596" s="1" t="s">
         <v>639</v>
       </c>
@@ -43625,7 +44168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="597" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="597" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A597" t="s">
         <v>640</v>
       </c>
@@ -43693,7 +44236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="598" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="598" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A598" s="1" t="s">
         <v>641</v>
       </c>
@@ -43761,7 +44304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="599" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="599" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A599" t="s">
         <v>642</v>
       </c>
@@ -43829,7 +44372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="600" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="600" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A600" s="1" t="s">
         <v>643</v>
       </c>
@@ -43897,7 +44440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="601" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="601" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A601" t="s">
         <v>644</v>
       </c>
@@ -43965,7 +44508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="602" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="602" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A602" s="1" t="s">
         <v>645</v>
       </c>
@@ -44030,10 +44573,13 @@
         <v>2</v>
       </c>
       <c r="W602" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="603" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="X602" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="603" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A603" t="s">
         <v>646</v>
       </c>
@@ -44100,8 +44646,11 @@
       <c r="W603" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="604" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X603" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="604" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A604" s="1" t="s">
         <v>647</v>
       </c>
@@ -44168,8 +44717,11 @@
       <c r="W604" s="1" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="605" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X604" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="605" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A605" t="s">
         <v>648</v>
       </c>
@@ -44236,8 +44788,11 @@
       <c r="W605" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="606" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X605" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="606" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A606" t="s">
         <v>649</v>
       </c>
@@ -44305,7 +44860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="607" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="607" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A607" s="1" t="s">
         <v>650</v>
       </c>
@@ -44373,7 +44928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="608" spans="1:23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="608" spans="1:24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A608" t="s">
         <v>651</v>
       </c>

</xml_diff>